<commit_message>
Issues #219 #222 fix for parsing integers & more than 26 columns in refactored excel code using OpenXml
</commit_message>
<xml_diff>
--- a/JosephM.CustomisationImporter.Test/TestCustomisationsUpdate.xlsx
+++ b/JosephM.CustomisationImporter.Test/TestCustomisationsUpdate.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joseph.mcgregor-macd\Source\Repos\XRM-Developer-Tool\JosephM.CustomisationImporter.Test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joseph.mcgregor-macd\source\repos\XRM-Developer-Tool\JosephM.CustomisationImporter.Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100"/>
   </bookViews>
   <sheets>
     <sheet name="Record Types" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="133">
   <si>
     <t>Record Type Schema Name</t>
   </si>
@@ -755,20 +755,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V21"/>
+  <dimension ref="A1:U21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" customWidth="1"/>
-    <col min="3" max="5" width="20.140625" customWidth="1"/>
-    <col min="6" max="22" width="7" customWidth="1"/>
-    <col min="23" max="26" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15.5546875" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" customWidth="1"/>
+    <col min="3" max="4" width="20.109375" customWidth="1"/>
+    <col min="5" max="21" width="7" customWidth="1"/>
+    <col min="22" max="25" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:21">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -785,26 +787,24 @@
         <v>8</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
@@ -814,9 +814,8 @@
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-    </row>
-    <row r="2" spans="1:22">
+    </row>
+    <row r="2" spans="1:21">
       <c r="A2" s="2" t="s">
         <v>27</v>
       </c>
@@ -829,14 +828,14 @@
       <c r="D2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="2" t="b">
+      <c r="E2" s="2">
         <v>0</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
       </c>
       <c r="G2" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2" s="2">
         <v>1</v>
@@ -850,11 +849,8 @@
       <c r="K2" s="2">
         <v>1</v>
       </c>
-      <c r="L2" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22">
+    </row>
+    <row r="3" spans="1:21">
       <c r="A3" s="2" t="s">
         <v>46</v>
       </c>
@@ -867,7 +863,7 @@
       <c r="D3" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="2" t="b">
+      <c r="E3" s="2">
         <v>0</v>
       </c>
       <c r="F3" s="2">
@@ -888,135 +884,114 @@
       <c r="K3" s="2">
         <v>0</v>
       </c>
-      <c r="L3" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22">
+    </row>
+    <row r="4" spans="1:21">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:22">
+    </row>
+    <row r="5" spans="1:21">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:22">
+    </row>
+    <row r="6" spans="1:21">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:22">
+    </row>
+    <row r="7" spans="1:21">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:22">
+    </row>
+    <row r="8" spans="1:21">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:22">
+    </row>
+    <row r="9" spans="1:21">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:22">
+    </row>
+    <row r="10" spans="1:21">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:22">
+    </row>
+    <row r="11" spans="1:21">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:22">
+    </row>
+    <row r="12" spans="1:21">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:22">
+    </row>
+    <row r="13" spans="1:21">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:22">
+    </row>
+    <row r="14" spans="1:21">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:22">
+    </row>
+    <row r="15" spans="1:21">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:22">
+    </row>
+    <row r="16" spans="1:21">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="1:5">
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="1:5">
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="1:5">
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="1:5">
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="1:5">
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1027,25 +1002,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="22.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" customWidth="1"/>
-    <col min="5" max="5" width="32.85546875" customWidth="1"/>
-    <col min="6" max="6" width="23.140625" customWidth="1"/>
-    <col min="7" max="11" width="19.7109375" customWidth="1"/>
-    <col min="12" max="13" width="13.7109375" customWidth="1"/>
-    <col min="14" max="17" width="12.7109375" customWidth="1"/>
-    <col min="18" max="18" width="11.5703125" customWidth="1"/>
-    <col min="19" max="20" width="11.42578125" customWidth="1"/>
-    <col min="21" max="21" width="39.42578125" customWidth="1"/>
-    <col min="22" max="22" width="6.140625" customWidth="1"/>
+    <col min="1" max="1" width="22.109375" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" customWidth="1"/>
+    <col min="5" max="5" width="32.88671875" customWidth="1"/>
+    <col min="6" max="6" width="23.109375" customWidth="1"/>
+    <col min="7" max="11" width="19.6640625" customWidth="1"/>
+    <col min="12" max="13" width="13.6640625" customWidth="1"/>
+    <col min="14" max="17" width="12.6640625" customWidth="1"/>
+    <col min="18" max="18" width="11.5546875" customWidth="1"/>
+    <col min="19" max="20" width="11.44140625" customWidth="1"/>
+    <col min="21" max="21" width="39.44140625" customWidth="1"/>
+    <col min="22" max="22" width="6.109375" customWidth="1"/>
     <col min="23" max="27" width="7" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7362,15 +7337,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
-    <col min="4" max="4" width="5.28515625" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="5.33203125" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" customWidth="1"/>
     <col min="6" max="15" width="7" customWidth="1"/>
-    <col min="16" max="26" width="12.5703125" customWidth="1"/>
+    <col min="16" max="26" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -7603,13 +7578,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="26.109375" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
     <col min="4" max="21" width="7" customWidth="1"/>
-    <col min="22" max="26" width="12.5703125" customWidth="1"/>
+    <col min="22" max="26" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">

</xml_diff>